<commit_message>
Updating some test models to comply with new xlsx and yml settings files structure. Working.
</commit_message>
<xml_diff>
--- a/tests/models/features/constants/input_data/input_data.xlsx
+++ b/tests/models/features/constants/input_data/input_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\units\constants\input_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\models\features\constants\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F0ECF4-904B-4435-A2CD-B4F76B9894F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FFC7B4-048C-4F80-8E3B-4366569D10D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24850" yWindow="3390" windowWidth="16140" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19680" yWindow="3420" windowWidth="14760" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Q" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <t>id</t>
   </si>
   <si>
-    <t>f_Name</t>
+    <t>flows_Name</t>
   </si>
   <si>
     <t>values</t>
@@ -409,7 +409,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>